<commit_message>
Changed in test method
</commit_message>
<xml_diff>
--- a/src/test/resources/student_registration.xlsx
+++ b/src/test/resources/student_registration.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ismedusoftsol-my.sharepoint.com/personal/ajangra_ismedusoftsol_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{63123A0B-69EF-4957-A449-3D785EBC22EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39725C9D-3F6A-48C2-9D65-3E5CE1D2F3EC}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{63123A0B-69EF-4957-A449-3D785EBC22EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDCB1EB3-6616-49FE-9AA7-1074DA06BC89}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{83E1AD02-E6B5-41C8-98D7-77709091ACEC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="2" xr2:uid="{83E1AD02-E6B5-41C8-98D7-77709091ACEC}"/>
   </bookViews>
   <sheets>
     <sheet name="studentData" sheetId="2" r:id="rId1"/>
-    <sheet name="employeeData" sheetId="3" r:id="rId2"/>
+    <sheet name="examManageData" sheetId="4" r:id="rId2"/>
+    <sheet name="subjectCreditData" sheetId="5" r:id="rId3"/>
+    <sheet name="employeeData" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="186">
   <si>
     <t>India</t>
   </si>
@@ -552,14 +554,43 @@
   </si>
   <si>
     <t>дети - инвалиды</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Academic Plan</t>
+  </si>
+  <si>
+    <t>Batch Field</t>
+  </si>
+  <si>
+    <t>Session Field</t>
+  </si>
+  <si>
+    <t>Semester Field</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>2026 -2027</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="24" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="76" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,8 +758,268 @@
       <sz val="11.0"/>
       <b val="true"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -911,6 +1202,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1111,7 +1408,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1128,20 +1425,234 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1526,7 +2037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B341502D-6CB3-4F48-AED9-FE9E3EEFEF78}">
   <dimension ref="A1:DS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+    <sheetView topLeftCell="AM1" workbookViewId="0">
       <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1659,364 +2170,364 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:123" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AA1" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AB1" s="118" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AD1" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AE1" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AF1" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AG1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AH1" s="118" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AJ1" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" s="12" t="s">
+      <c r="AK1" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AL1" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AM1" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AN1" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AO1" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AP1" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+      <c r="AQ1" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="AR1" s="12" t="s">
+      <c r="AR1" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="AS1" s="12" t="s">
+      <c r="AS1" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="AT1" s="12" t="s">
+      <c r="AT1" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="AU1" s="12" t="s">
+      <c r="AU1" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AV1" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="AW1" s="12" t="s">
+      <c r="AW1" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="AX1" s="12" t="s">
+      <c r="AX1" s="118" t="s">
         <v>53</v>
       </c>
-      <c r="AY1" s="12" t="s">
+      <c r="AY1" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="AZ1" s="12" t="s">
+      <c r="AZ1" s="118" t="s">
         <v>55</v>
       </c>
-      <c r="BA1" s="12" t="s">
+      <c r="BA1" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="BB1" s="12" t="s">
+      <c r="BB1" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="BC1" s="12" t="s">
+      <c r="BC1" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="BD1" s="12" t="s">
+      <c r="BD1" s="118" t="s">
         <v>59</v>
       </c>
-      <c r="BE1" s="12" t="s">
+      <c r="BE1" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="BF1" s="12" t="s">
+      <c r="BF1" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="BG1" s="12" t="s">
+      <c r="BG1" s="118" t="s">
         <v>62</v>
       </c>
-      <c r="BH1" s="12" t="s">
+      <c r="BH1" s="118" t="s">
         <v>63</v>
       </c>
-      <c r="BI1" s="12" t="s">
+      <c r="BI1" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="BJ1" s="12" t="s">
+      <c r="BJ1" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="BK1" s="12" t="s">
+      <c r="BK1" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="BL1" s="12" t="s">
+      <c r="BL1" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="BM1" s="12" t="s">
+      <c r="BM1" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="BN1" s="12" t="s">
+      <c r="BN1" s="118" t="s">
         <v>69</v>
       </c>
-      <c r="BO1" s="12" t="s">
+      <c r="BO1" s="118" t="s">
         <v>70</v>
       </c>
-      <c r="BP1" s="12" t="s">
+      <c r="BP1" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="BQ1" s="12" t="s">
+      <c r="BQ1" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="BR1" s="12" t="s">
+      <c r="BR1" s="118" t="s">
         <v>73</v>
       </c>
-      <c r="BS1" s="12" t="s">
+      <c r="BS1" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="BT1" s="12" t="s">
+      <c r="BT1" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="BU1" s="12" t="s">
+      <c r="BU1" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="BV1" s="12" t="s">
+      <c r="BV1" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="BW1" s="12" t="s">
+      <c r="BW1" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="BX1" s="12" t="s">
+      <c r="BX1" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="BY1" s="12" t="s">
+      <c r="BY1" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="BZ1" s="12" t="s">
+      <c r="BZ1" s="118" t="s">
         <v>81</v>
       </c>
-      <c r="CA1" s="12" t="s">
+      <c r="CA1" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="CB1" s="12" t="s">
+      <c r="CB1" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="CC1" s="12" t="s">
+      <c r="CC1" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="CD1" s="12" t="s">
+      <c r="CD1" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="CE1" s="12" t="s">
+      <c r="CE1" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="CF1" s="12" t="s">
+      <c r="CF1" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="CG1" s="12" t="s">
+      <c r="CG1" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="CH1" s="12" t="s">
+      <c r="CH1" s="118" t="s">
         <v>89</v>
       </c>
-      <c r="CI1" s="12" t="s">
+      <c r="CI1" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="CJ1" s="12" t="s">
+      <c r="CJ1" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="CK1" s="12" t="s">
+      <c r="CK1" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="CL1" s="12" t="s">
+      <c r="CL1" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="CM1" s="12" t="s">
+      <c r="CM1" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="CN1" s="12" t="s">
+      <c r="CN1" s="118" t="s">
         <v>95</v>
       </c>
-      <c r="CO1" s="12" t="s">
+      <c r="CO1" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="CP1" s="12" t="s">
+      <c r="CP1" s="118" t="s">
         <v>97</v>
       </c>
-      <c r="CQ1" s="12" t="s">
+      <c r="CQ1" s="118" t="s">
         <v>98</v>
       </c>
-      <c r="CR1" s="12" t="s">
+      <c r="CR1" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="CS1" s="12" t="s">
+      <c r="CS1" s="118" t="s">
         <v>100</v>
       </c>
-      <c r="CT1" s="12" t="s">
+      <c r="CT1" s="118" t="s">
         <v>101</v>
       </c>
-      <c r="CU1" s="12" t="s">
+      <c r="CU1" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="CV1" s="12" t="s">
+      <c r="CV1" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="CW1" s="12" t="s">
+      <c r="CW1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="CX1" s="12" t="s">
+      <c r="CX1" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="CY1" s="12" t="s">
+      <c r="CY1" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="CZ1" s="12" t="s">
+      <c r="CZ1" s="118" t="s">
         <v>105</v>
       </c>
-      <c r="DA1" s="12" t="s">
+      <c r="DA1" s="118" t="s">
         <v>106</v>
       </c>
-      <c r="DB1" s="12" t="s">
+      <c r="DB1" s="118" t="s">
         <v>107</v>
       </c>
-      <c r="DC1" s="12" t="s">
+      <c r="DC1" s="118" t="s">
         <v>108</v>
       </c>
-      <c r="DD1" s="12" t="s">
+      <c r="DD1" s="118" t="s">
         <v>109</v>
       </c>
-      <c r="DE1" s="12" t="s">
+      <c r="DE1" s="118" t="s">
         <v>110</v>
       </c>
-      <c r="DF1" s="12" t="s">
+      <c r="DF1" s="118" t="s">
         <v>111</v>
       </c>
-      <c r="DG1" s="12" t="s">
+      <c r="DG1" s="118" t="s">
         <v>112</v>
       </c>
-      <c r="DH1" s="12" t="s">
+      <c r="DH1" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="DI1" s="12" t="s">
+      <c r="DI1" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="DJ1" s="12" t="s">
+      <c r="DJ1" s="118" t="s">
         <v>115</v>
       </c>
-      <c r="DK1" s="12" t="s">
+      <c r="DK1" s="118" t="s">
         <v>116</v>
       </c>
-      <c r="DL1" s="12" t="s">
+      <c r="DL1" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="DM1" s="12" t="s">
+      <c r="DM1" s="118" t="s">
         <v>118</v>
       </c>
-      <c r="DN1" s="12" t="s">
+      <c r="DN1" s="118" t="s">
         <v>119</v>
       </c>
-      <c r="DO1" s="12" t="s">
+      <c r="DO1" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="DP1" s="12" t="s">
+      <c r="DP1" s="118" t="s">
         <v>121</v>
       </c>
       <c r="DQ1" s="4" t="s">
@@ -2384,7 +2895,7 @@
       <c r="DN2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="DO2" s="13" t="s">
+      <c r="DO2" s="119" t="s">
         <v>159</v>
       </c>
       <c r="DP2" s="2">
@@ -2410,6 +2921,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F61D5DF-4A16-4FA1-BA8E-05C7CD8F33F9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.6640625"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="10.33203125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>46092</v>
+      </c>
+      <c r="D2" s="7">
+        <v>46094</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14472D50-E132-4C29-8AF0-3B323C0246C9}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.88671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.88671875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.5546875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25EAF2F-9178-45A3-8457-26D257E3A99A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changed in the test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/student_registration.xlsx
+++ b/src/test/resources/student_registration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="186">
   <si>
     <t>India</t>
   </si>
@@ -590,7 +590,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="76" x14ac:knownFonts="1">
+  <fonts count="88" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,6 +737,66 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1408,7 +1468,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1652,6 +1712,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="75" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="36" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2170,364 +2278,364 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:123" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="142" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="142" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="118" t="s">
+      <c r="H1" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="118" t="s">
+      <c r="I1" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="118" t="s">
+      <c r="J1" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="118" t="s">
+      <c r="K1" s="142" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="118" t="s">
+      <c r="L1" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="118" t="s">
+      <c r="M1" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="118" t="s">
+      <c r="N1" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="118" t="s">
+      <c r="O1" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="118" t="s">
+      <c r="P1" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="118" t="s">
+      <c r="Q1" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="118" t="s">
+      <c r="R1" s="142" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="118" t="s">
+      <c r="S1" s="142" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="118" t="s">
+      <c r="T1" s="142" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="118" t="s">
+      <c r="U1" s="142" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="118" t="s">
+      <c r="V1" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="118" t="s">
+      <c r="W1" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="118" t="s">
+      <c r="X1" s="142" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="118" t="s">
+      <c r="Y1" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="118" t="s">
+      <c r="Z1" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="118" t="s">
+      <c r="AA1" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" s="118" t="s">
+      <c r="AB1" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="118" t="s">
+      <c r="AC1" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" s="118" t="s">
+      <c r="AD1" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" s="118" t="s">
+      <c r="AE1" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" s="118" t="s">
+      <c r="AF1" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="118" t="s">
+      <c r="AG1" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" s="118" t="s">
+      <c r="AH1" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" s="118" t="s">
+      <c r="AI1" s="142" t="s">
         <v>38</v>
       </c>
-      <c r="AJ1" s="118" t="s">
+      <c r="AJ1" s="142" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" s="118" t="s">
+      <c r="AK1" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="AL1" s="118" t="s">
+      <c r="AL1" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="AM1" s="118" t="s">
+      <c r="AM1" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="AN1" s="118" t="s">
+      <c r="AN1" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="AO1" s="118" t="s">
+      <c r="AO1" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="AP1" s="118" t="s">
+      <c r="AP1" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="AQ1" s="118" t="s">
+      <c r="AQ1" s="142" t="s">
         <v>46</v>
       </c>
-      <c r="AR1" s="118" t="s">
+      <c r="AR1" s="142" t="s">
         <v>47</v>
       </c>
-      <c r="AS1" s="118" t="s">
+      <c r="AS1" s="142" t="s">
         <v>48</v>
       </c>
-      <c r="AT1" s="118" t="s">
+      <c r="AT1" s="142" t="s">
         <v>49</v>
       </c>
-      <c r="AU1" s="118" t="s">
+      <c r="AU1" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="AV1" s="118" t="s">
+      <c r="AV1" s="142" t="s">
         <v>51</v>
       </c>
-      <c r="AW1" s="118" t="s">
+      <c r="AW1" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="AX1" s="118" t="s">
+      <c r="AX1" s="142" t="s">
         <v>53</v>
       </c>
-      <c r="AY1" s="118" t="s">
+      <c r="AY1" s="142" t="s">
         <v>54</v>
       </c>
-      <c r="AZ1" s="118" t="s">
+      <c r="AZ1" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="BA1" s="118" t="s">
+      <c r="BA1" s="142" t="s">
         <v>56</v>
       </c>
-      <c r="BB1" s="118" t="s">
+      <c r="BB1" s="142" t="s">
         <v>57</v>
       </c>
-      <c r="BC1" s="118" t="s">
+      <c r="BC1" s="142" t="s">
         <v>58</v>
       </c>
-      <c r="BD1" s="118" t="s">
+      <c r="BD1" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="BE1" s="118" t="s">
+      <c r="BE1" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="BF1" s="118" t="s">
+      <c r="BF1" s="142" t="s">
         <v>61</v>
       </c>
-      <c r="BG1" s="118" t="s">
+      <c r="BG1" s="142" t="s">
         <v>62</v>
       </c>
-      <c r="BH1" s="118" t="s">
+      <c r="BH1" s="142" t="s">
         <v>63</v>
       </c>
-      <c r="BI1" s="118" t="s">
+      <c r="BI1" s="142" t="s">
         <v>64</v>
       </c>
-      <c r="BJ1" s="118" t="s">
+      <c r="BJ1" s="142" t="s">
         <v>65</v>
       </c>
-      <c r="BK1" s="118" t="s">
+      <c r="BK1" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="BL1" s="118" t="s">
+      <c r="BL1" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="BM1" s="118" t="s">
+      <c r="BM1" s="142" t="s">
         <v>68</v>
       </c>
-      <c r="BN1" s="118" t="s">
+      <c r="BN1" s="142" t="s">
         <v>69</v>
       </c>
-      <c r="BO1" s="118" t="s">
+      <c r="BO1" s="142" t="s">
         <v>70</v>
       </c>
-      <c r="BP1" s="118" t="s">
+      <c r="BP1" s="142" t="s">
         <v>71</v>
       </c>
-      <c r="BQ1" s="118" t="s">
+      <c r="BQ1" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="BR1" s="118" t="s">
+      <c r="BR1" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="BS1" s="118" t="s">
+      <c r="BS1" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="BT1" s="118" t="s">
+      <c r="BT1" s="142" t="s">
         <v>75</v>
       </c>
-      <c r="BU1" s="118" t="s">
+      <c r="BU1" s="142" t="s">
         <v>76</v>
       </c>
-      <c r="BV1" s="118" t="s">
+      <c r="BV1" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="BW1" s="118" t="s">
+      <c r="BW1" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="BX1" s="118" t="s">
+      <c r="BX1" s="142" t="s">
         <v>79</v>
       </c>
-      <c r="BY1" s="118" t="s">
+      <c r="BY1" s="142" t="s">
         <v>80</v>
       </c>
-      <c r="BZ1" s="118" t="s">
+      <c r="BZ1" s="142" t="s">
         <v>81</v>
       </c>
-      <c r="CA1" s="118" t="s">
+      <c r="CA1" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="CB1" s="118" t="s">
+      <c r="CB1" s="142" t="s">
         <v>83</v>
       </c>
-      <c r="CC1" s="118" t="s">
+      <c r="CC1" s="142" t="s">
         <v>84</v>
       </c>
-      <c r="CD1" s="118" t="s">
+      <c r="CD1" s="142" t="s">
         <v>85</v>
       </c>
-      <c r="CE1" s="118" t="s">
+      <c r="CE1" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="CF1" s="118" t="s">
+      <c r="CF1" s="142" t="s">
         <v>87</v>
       </c>
-      <c r="CG1" s="118" t="s">
+      <c r="CG1" s="142" t="s">
         <v>88</v>
       </c>
-      <c r="CH1" s="118" t="s">
+      <c r="CH1" s="142" t="s">
         <v>89</v>
       </c>
-      <c r="CI1" s="118" t="s">
+      <c r="CI1" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="CJ1" s="118" t="s">
+      <c r="CJ1" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="CK1" s="118" t="s">
+      <c r="CK1" s="142" t="s">
         <v>92</v>
       </c>
-      <c r="CL1" s="118" t="s">
+      <c r="CL1" s="142" t="s">
         <v>93</v>
       </c>
-      <c r="CM1" s="118" t="s">
+      <c r="CM1" s="142" t="s">
         <v>94</v>
       </c>
-      <c r="CN1" s="118" t="s">
+      <c r="CN1" s="142" t="s">
         <v>95</v>
       </c>
-      <c r="CO1" s="118" t="s">
+      <c r="CO1" s="142" t="s">
         <v>96</v>
       </c>
-      <c r="CP1" s="118" t="s">
+      <c r="CP1" s="142" t="s">
         <v>97</v>
       </c>
-      <c r="CQ1" s="118" t="s">
+      <c r="CQ1" s="142" t="s">
         <v>98</v>
       </c>
-      <c r="CR1" s="118" t="s">
+      <c r="CR1" s="142" t="s">
         <v>99</v>
       </c>
-      <c r="CS1" s="118" t="s">
+      <c r="CS1" s="142" t="s">
         <v>100</v>
       </c>
-      <c r="CT1" s="118" t="s">
+      <c r="CT1" s="142" t="s">
         <v>101</v>
       </c>
-      <c r="CU1" s="118" t="s">
+      <c r="CU1" s="142" t="s">
         <v>102</v>
       </c>
-      <c r="CV1" s="118" t="s">
+      <c r="CV1" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="CW1" s="118" t="s">
+      <c r="CW1" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="CX1" s="118" t="s">
+      <c r="CX1" s="142" t="s">
         <v>103</v>
       </c>
-      <c r="CY1" s="118" t="s">
+      <c r="CY1" s="142" t="s">
         <v>104</v>
       </c>
-      <c r="CZ1" s="118" t="s">
+      <c r="CZ1" s="142" t="s">
         <v>105</v>
       </c>
-      <c r="DA1" s="118" t="s">
+      <c r="DA1" s="142" t="s">
         <v>106</v>
       </c>
-      <c r="DB1" s="118" t="s">
+      <c r="DB1" s="142" t="s">
         <v>107</v>
       </c>
-      <c r="DC1" s="118" t="s">
+      <c r="DC1" s="142" t="s">
         <v>108</v>
       </c>
-      <c r="DD1" s="118" t="s">
+      <c r="DD1" s="142" t="s">
         <v>109</v>
       </c>
-      <c r="DE1" s="118" t="s">
+      <c r="DE1" s="142" t="s">
         <v>110</v>
       </c>
-      <c r="DF1" s="118" t="s">
+      <c r="DF1" s="142" t="s">
         <v>111</v>
       </c>
-      <c r="DG1" s="118" t="s">
+      <c r="DG1" s="142" t="s">
         <v>112</v>
       </c>
-      <c r="DH1" s="118" t="s">
+      <c r="DH1" s="142" t="s">
         <v>113</v>
       </c>
-      <c r="DI1" s="118" t="s">
+      <c r="DI1" s="142" t="s">
         <v>114</v>
       </c>
-      <c r="DJ1" s="118" t="s">
+      <c r="DJ1" s="142" t="s">
         <v>115</v>
       </c>
-      <c r="DK1" s="118" t="s">
+      <c r="DK1" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="DL1" s="118" t="s">
+      <c r="DL1" s="142" t="s">
         <v>117</v>
       </c>
-      <c r="DM1" s="118" t="s">
+      <c r="DM1" s="142" t="s">
         <v>118</v>
       </c>
-      <c r="DN1" s="118" t="s">
+      <c r="DN1" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="DO1" s="118" t="s">
+      <c r="DO1" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="DP1" s="118" t="s">
+      <c r="DP1" s="142" t="s">
         <v>121</v>
       </c>
       <c r="DQ1" s="4" t="s">
@@ -2895,7 +3003,7 @@
       <c r="DN2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="DO2" s="119" t="s">
+      <c r="DO2" s="143" t="s">
         <v>159</v>
       </c>
       <c r="DP2" s="2">

</xml_diff>